<commit_message>
!!! NONE vs 0 !!!
</commit_message>
<xml_diff>
--- a/football_stats.xlsx
+++ b/football_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\football_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2A3FFA-208D-482C-9B27-E12B3102B86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB19605-0501-457B-B9C3-F42D18667428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="0" windowWidth="15120" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,80 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -586,38 +658,32 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -746,13 +812,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -772,109 +831,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -882,10 +839,7 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -894,12 +848,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -940,6 +888,58 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1017,18 +1017,18 @@
     <sortCondition descending="1" ref="F1:F54"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72D5507B-3E56-45F9-949A-1B810B89614D}" name="player_id" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9B600E03-F10C-49A9-BD9C-050BEA58FF6E}" name="player_name" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{8F857898-2667-4829-90AD-3A28B8E44AF3}" name="goals" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{72D5507B-3E56-45F9-949A-1B810B89614D}" name="player_id" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{9B600E03-F10C-49A9-BD9C-050BEA58FF6E}" name="player_name" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{8F857898-2667-4829-90AD-3A28B8E44AF3}" name="goals" dataDxfId="23">
       <calculatedColumnFormula>SUMIFS(_stats[goals_on_date],_stats[player_id],_players[[#This Row],[player_id]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{81B9F6B2-D5CC-4D13-9EE3-73B39091AD58}" name="assists" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{81B9F6B2-D5CC-4D13-9EE3-73B39091AD58}" name="assists" dataDxfId="22">
       <calculatedColumnFormula>SUMIFS(_stats[assists_on_date],_stats[player_id],_players[[#This Row],[player_id]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1C26950D-761D-4C94-B228-1824773DE1A0}" name="wins" dataDxfId="24">
+    <tableColumn id="5" xr3:uid="{1C26950D-761D-4C94-B228-1824773DE1A0}" name="wins" dataDxfId="21">
       <calculatedColumnFormula>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9ADB0D0F-407B-4516-A8B8-97C920F43BB4}" name="points" dataDxfId="23">
+    <tableColumn id="6" xr3:uid="{9ADB0D0F-407B-4516-A8B8-97C920F43BB4}" name="points" dataDxfId="20">
       <calculatedColumnFormula>SUM(_players[[#This Row],[goals]:[wins]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1037,21 +1037,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3D1149F-12DA-4A23-97C8-9D9CCA1140FB}" name="_stats" displayName="_stats" ref="A1:G89" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3D1149F-12DA-4A23-97C8-9D9CCA1140FB}" name="_stats" displayName="_stats" ref="A1:G89" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:G89" xr:uid="{D3D1149F-12DA-4A23-97C8-9D9CCA1140FB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G60">
     <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D6DD79FC-E04C-45EB-8EBE-D6811A0C69D0}" name="date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{686C940A-87F8-43A1-ADFF-9CF607E801B5}" name="team_number" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{1C13D6CA-8B0C-4849-B32C-A77EF9C52B42}" name="player_id" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C2384479-71AA-40DA-A7B2-E30ECBA1AF99}" name="player_name" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{D6DD79FC-E04C-45EB-8EBE-D6811A0C69D0}" name="date" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{686C940A-87F8-43A1-ADFF-9CF607E801B5}" name="team_number" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{1C13D6CA-8B0C-4849-B32C-A77EF9C52B42}" name="player_id" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{C2384479-71AA-40DA-A7B2-E30ECBA1AF99}" name="player_name" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{09AE1D8B-DCB8-4F87-ABB5-372822B0D6BF}" name="goals_on_date" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{7FD24496-81EB-47BB-8B89-26AB97C686CA}" name="assists_on_date" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{39F202A0-49EF-45EE-9054-882F18FBDF31}" name="wins_on_date" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{09AE1D8B-DCB8-4F87-ABB5-372822B0D6BF}" name="goals_on_date" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{7FD24496-81EB-47BB-8B89-26AB97C686CA}" name="assists_on_date" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{39F202A0-49EF-45EE-9054-882F18FBDF31}" name="wins_on_date" dataDxfId="8">
       <calculatedColumnFormula>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1060,12 +1060,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B6423DC2-EC3F-4914-9E08-BC4E7C6626C9}" name="_teams" displayName="_teams" ref="A1:C14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B6423DC2-EC3F-4914-9E08-BC4E7C6626C9}" name="_teams" displayName="_teams" ref="A1:C14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C14" xr:uid="{B6423DC2-EC3F-4914-9E08-BC4E7C6626C9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{92BE0DCE-EF0C-43B2-937D-640EBFF087A6}" name="date" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{B497FB59-180E-4B72-9ECD-E25C88173489}" name="team_number" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{02A8A062-9D85-4980-948F-E89B2B2D08DF}" name="wins_on_date" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{92BE0DCE-EF0C-43B2-937D-640EBFF087A6}" name="date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{B497FB59-180E-4B72-9ECD-E25C88173489}" name="team_number" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{02A8A062-9D85-4980-948F-E89B2B2D08DF}" name="wins_on_date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1339,8 +1339,8 @@
   </sheetPr>
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,8 +2661,8 @@
   </sheetPr>
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,8 +2712,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Женя (кипер)</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
       <c r="G2" s="8">
         <v>2</v>
       </c>
@@ -2732,7 +2736,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Толя Шлаев</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
       <c r="F3" s="9">
         <v>2</v>
       </c>
@@ -2757,7 +2763,9 @@
       <c r="E4" s="8">
         <v>2</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
       <c r="G4" s="8">
         <v>2</v>
       </c>
@@ -2776,8 +2784,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Тёма</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
       <c r="G5" s="8">
         <v>4</v>
       </c>
@@ -2799,7 +2811,9 @@
       <c r="E6" s="8">
         <v>1</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
       <c r="G6" s="8">
         <v>2</v>
       </c>
@@ -2818,7 +2832,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Максим Строцкий</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
       <c r="F7" s="9">
         <v>3</v>
       </c>
@@ -2840,8 +2856,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Василий Улитин</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
       <c r="G8" s="8">
         <v>2</v>
       </c>
@@ -2884,7 +2904,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Александр</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
       <c r="F10" s="9">
         <v>1</v>
       </c>
@@ -2933,7 +2955,9 @@
       <c r="E12" s="8">
         <v>2</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
       <c r="G12" s="8">
         <v>4</v>
       </c>
@@ -2976,8 +3000,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Руслан (от Сергея)</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
       <c r="G14" s="8">
         <v>2</v>
       </c>
@@ -2996,7 +3024,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Расул</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
       <c r="F15" s="9">
         <v>2</v>
       </c>
@@ -3090,7 +3120,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Никита</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
       <c r="F19" s="9">
         <v>1</v>
       </c>
@@ -3112,8 +3144,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Миша</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
       <c r="G20" s="8">
         <v>1</v>
       </c>
@@ -3156,8 +3192,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Bu (Рыжий)</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
       <c r="G22" s="8">
         <v>1</v>
       </c>
@@ -3179,7 +3219,9 @@
       <c r="E23" s="8">
         <v>1</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
       <c r="G23" s="8">
         <v>3</v>
       </c>
@@ -3198,8 +3240,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Александр Травкин</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
       <c r="G24" s="8">
         <v>1</v>
       </c>
@@ -3218,7 +3264,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Олег Шишкин</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
       <c r="F25" s="9">
         <v>1</v>
       </c>
@@ -3240,8 +3288,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Женя (кипер)</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
       <c r="G26" s="8">
         <v>3</v>
       </c>
@@ -3260,8 +3312,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Сергей</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
       <c r="G27" s="8">
         <v>1</v>
       </c>
@@ -3283,7 +3339,9 @@
       <c r="E28" s="8">
         <v>1</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
       <c r="G28" s="8">
         <v>5</v>
       </c>
@@ -3329,7 +3387,9 @@
       <c r="E30" s="8">
         <v>1</v>
       </c>
-      <c r="F30" s="9"/>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
       <c r="G30" s="8">
         <v>3</v>
       </c>
@@ -3348,7 +3408,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Сергей Крюков</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
       <c r="F31" s="9">
         <v>1</v>
       </c>
@@ -3370,8 +3432,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Рома Сурнин</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+      <c r="F32" s="9">
+        <v>0</v>
+      </c>
       <c r="G32" s="8">
         <v>3</v>
       </c>
@@ -3390,8 +3456,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Дядя Руслан</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
+      <c r="E33" s="8">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
       <c r="G33" s="8">
         <v>5</v>
       </c>
@@ -3410,8 +3480,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Женя Одушкин</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
+      <c r="E34" s="8">
+        <v>0</v>
+      </c>
+      <c r="F34" s="9">
+        <v>0</v>
+      </c>
       <c r="G34" s="8">
         <v>1</v>
       </c>
@@ -3430,7 +3504,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Эд (Сэм)</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
       <c r="F35" s="9">
         <v>1</v>
       </c>
@@ -3452,8 +3528,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Рубик</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="9"/>
+      <c r="E36" s="8">
+        <v>0</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
       <c r="G36" s="8">
         <v>3</v>
       </c>
@@ -3472,8 +3552,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Рубик +1</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="9"/>
+      <c r="E37" s="8">
+        <v>0</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
       <c r="G37" s="8">
         <v>3</v>
       </c>
@@ -3492,8 +3576,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Артем Ширяев</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="9"/>
+      <c r="E38" s="8">
+        <v>0</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0</v>
+      </c>
       <c r="G38" s="8">
         <v>1</v>
       </c>
@@ -3512,8 +3600,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Ваня</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
+      <c r="E39" s="8">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0</v>
+      </c>
       <c r="G39" s="8">
         <v>1</v>
       </c>
@@ -3535,7 +3627,9 @@
       <c r="E40" s="8">
         <v>1</v>
       </c>
-      <c r="F40" s="9"/>
+      <c r="F40" s="9">
+        <v>0</v>
+      </c>
       <c r="G40" s="8">
         <v>5</v>
       </c>
@@ -3554,8 +3648,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Нурик</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
+      <c r="E41" s="8">
+        <v>0</v>
+      </c>
+      <c r="F41" s="9">
+        <v>0</v>
+      </c>
       <c r="G41" s="8">
         <v>7</v>
       </c>
@@ -3622,7 +3720,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Расул</v>
       </c>
-      <c r="E44" s="8"/>
+      <c r="E44" s="8">
+        <v>0</v>
+      </c>
       <c r="F44" s="9">
         <v>1</v>
       </c>
@@ -3668,7 +3768,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Тёма</v>
       </c>
-      <c r="E46" s="8"/>
+      <c r="E46" s="8">
+        <v>0</v>
+      </c>
       <c r="F46" s="9">
         <v>2</v>
       </c>
@@ -3690,8 +3792,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Никита</v>
       </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="9"/>
+      <c r="E47" s="8">
+        <v>0</v>
+      </c>
+      <c r="F47" s="9">
+        <v>0</v>
+      </c>
       <c r="G47" s="8">
         <v>1</v>
       </c>
@@ -3710,8 +3816,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Женя (кипер)</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="9"/>
+      <c r="E48" s="8">
+        <v>0</v>
+      </c>
+      <c r="F48" s="9">
+        <v>0</v>
+      </c>
       <c r="G48" s="8">
         <v>1</v>
       </c>
@@ -3778,7 +3888,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Влад</v>
       </c>
-      <c r="E51" s="8"/>
+      <c r="E51" s="8">
+        <v>0</v>
+      </c>
       <c r="F51" s="9">
         <v>1</v>
       </c>
@@ -3824,8 +3936,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Сергей Крюков</v>
       </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="9"/>
+      <c r="E53" s="8">
+        <v>0</v>
+      </c>
+      <c r="F53" s="9">
+        <v>0</v>
+      </c>
       <c r="G53" s="8">
         <v>7</v>
       </c>
@@ -3844,8 +3960,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Стас (от Расула)</v>
       </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="9"/>
+      <c r="E54" s="8">
+        <v>0</v>
+      </c>
+      <c r="F54" s="9">
+        <v>0</v>
+      </c>
       <c r="G54" s="8">
         <v>1</v>
       </c>
@@ -3867,7 +3987,9 @@
       <c r="E55" s="8">
         <v>1</v>
       </c>
-      <c r="F55" s="9"/>
+      <c r="F55" s="9">
+        <v>0</v>
+      </c>
       <c r="G55" s="8">
         <v>1</v>
       </c>
@@ -3910,8 +4032,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Атай</v>
       </c>
-      <c r="E57" s="8"/>
-      <c r="F57" s="9"/>
+      <c r="E57" s="8">
+        <v>0</v>
+      </c>
+      <c r="F57" s="9">
+        <v>0</v>
+      </c>
       <c r="G57" s="8">
         <v>1</v>
       </c>
@@ -3954,7 +4080,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Олег Шишкин</v>
       </c>
-      <c r="E59" s="8"/>
+      <c r="E59" s="8">
+        <v>0</v>
+      </c>
       <c r="F59" s="9">
         <v>1</v>
       </c>
@@ -3976,8 +4104,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Месси (от Расула)</v>
       </c>
-      <c r="E60" s="8"/>
-      <c r="F60" s="9"/>
+      <c r="E60" s="8">
+        <v>0</v>
+      </c>
+      <c r="F60" s="9">
+        <v>0</v>
+      </c>
       <c r="G60" s="8">
         <v>1</v>
       </c>
@@ -4020,8 +4152,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Артем Ширяев</v>
       </c>
-      <c r="E62" s="26"/>
-      <c r="F62" s="28"/>
+      <c r="E62" s="26">
+        <v>0</v>
+      </c>
+      <c r="F62" s="28">
+        <v>0</v>
+      </c>
       <c r="G62" s="27">
         <v>6</v>
       </c>
@@ -4088,8 +4224,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Никита</v>
       </c>
-      <c r="E65" s="26"/>
-      <c r="F65" s="28"/>
+      <c r="E65" s="26">
+        <v>0</v>
+      </c>
+      <c r="F65" s="28">
+        <v>0</v>
+      </c>
       <c r="G65" s="27">
         <v>4</v>
       </c>
@@ -4108,8 +4248,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Олег Шишкин</v>
       </c>
-      <c r="E66" s="26"/>
-      <c r="F66" s="28"/>
+      <c r="E66" s="26">
+        <v>0</v>
+      </c>
+      <c r="F66" s="28">
+        <v>0</v>
+      </c>
       <c r="G66" s="27">
         <v>6</v>
       </c>
@@ -4176,8 +4320,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Тёма</v>
       </c>
-      <c r="E69" s="26"/>
-      <c r="F69" s="28"/>
+      <c r="E69" s="26">
+        <v>0</v>
+      </c>
+      <c r="F69" s="28">
+        <v>0</v>
+      </c>
       <c r="G69" s="27">
         <v>6</v>
       </c>
@@ -4220,8 +4368,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Женя (кипер)</v>
       </c>
-      <c r="E71" s="26"/>
-      <c r="F71" s="28"/>
+      <c r="E71" s="26">
+        <v>0</v>
+      </c>
+      <c r="F71" s="28">
+        <v>0</v>
+      </c>
       <c r="G71" s="27">
         <v>4</v>
       </c>
@@ -4240,7 +4392,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Андрей (АК+1)</v>
       </c>
-      <c r="E72" s="26"/>
+      <c r="E72" s="26">
+        <v>0</v>
+      </c>
       <c r="F72" s="28">
         <v>1</v>
       </c>
@@ -4265,7 +4419,9 @@
       <c r="E73" s="26">
         <v>2</v>
       </c>
-      <c r="F73" s="28"/>
+      <c r="F73" s="28">
+        <v>0</v>
+      </c>
       <c r="G73" s="27">
         <v>2</v>
       </c>
@@ -4284,8 +4440,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Кирилл (АК+1)</v>
       </c>
-      <c r="E74" s="26"/>
-      <c r="F74" s="28"/>
+      <c r="E74" s="26">
+        <v>0</v>
+      </c>
+      <c r="F74" s="28">
+        <v>0</v>
+      </c>
       <c r="G74" s="27">
         <v>2</v>
       </c>
@@ -4304,8 +4464,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Илья (АК+1)</v>
       </c>
-      <c r="E75" s="26"/>
-      <c r="F75" s="28"/>
+      <c r="E75" s="26">
+        <v>0</v>
+      </c>
+      <c r="F75" s="28">
+        <v>0</v>
+      </c>
       <c r="G75" s="27">
         <v>2</v>
       </c>
@@ -4324,8 +4488,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Рамиль (АК+1)</v>
       </c>
-      <c r="E76" s="26"/>
-      <c r="F76" s="28"/>
+      <c r="E76" s="26">
+        <v>0</v>
+      </c>
+      <c r="F76" s="28">
+        <v>0</v>
+      </c>
       <c r="G76" s="27">
         <v>2</v>
       </c>
@@ -4347,7 +4515,9 @@
       <c r="E77" s="26">
         <v>1</v>
       </c>
-      <c r="F77" s="28"/>
+      <c r="F77" s="28">
+        <v>0</v>
+      </c>
       <c r="G77" s="27">
         <v>4</v>
       </c>
@@ -4369,7 +4539,9 @@
       <c r="E78" s="26">
         <v>1</v>
       </c>
-      <c r="F78" s="28"/>
+      <c r="F78" s="28">
+        <v>0</v>
+      </c>
       <c r="G78" s="27">
         <v>0</v>
       </c>
@@ -4388,8 +4560,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Сома (Руб)</v>
       </c>
-      <c r="E79" s="26"/>
-      <c r="F79" s="28"/>
+      <c r="E79" s="26">
+        <v>0</v>
+      </c>
+      <c r="F79" s="28">
+        <v>0</v>
+      </c>
       <c r="G79" s="27">
         <v>0</v>
       </c>
@@ -4411,7 +4587,9 @@
       <c r="E80" s="26">
         <v>2</v>
       </c>
-      <c r="F80" s="28"/>
+      <c r="F80" s="28">
+        <v>0</v>
+      </c>
       <c r="G80" s="27">
         <v>4</v>
       </c>
@@ -4430,7 +4608,9 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Дима (Руб)</v>
       </c>
-      <c r="E81" s="26"/>
+      <c r="E81" s="26">
+        <v>0</v>
+      </c>
       <c r="F81" s="28">
         <v>1</v>
       </c>
@@ -4452,8 +4632,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Юра Пименов</v>
       </c>
-      <c r="E82" s="26"/>
-      <c r="F82" s="28"/>
+      <c r="E82" s="26">
+        <v>0</v>
+      </c>
+      <c r="F82" s="28">
+        <v>0</v>
+      </c>
       <c r="G82" s="27">
         <v>6</v>
       </c>
@@ -4472,8 +4656,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Игорь Фомичев</v>
       </c>
-      <c r="E83" s="26"/>
-      <c r="F83" s="28"/>
+      <c r="E83" s="26">
+        <v>0</v>
+      </c>
+      <c r="F83" s="28">
+        <v>0</v>
+      </c>
       <c r="G83" s="27">
         <v>6</v>
       </c>
@@ -4516,8 +4704,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Миша (АК+1)</v>
       </c>
-      <c r="E85" s="26"/>
-      <c r="F85" s="28"/>
+      <c r="E85" s="26">
+        <v>0</v>
+      </c>
+      <c r="F85" s="28">
+        <v>0</v>
+      </c>
       <c r="G85" s="27">
         <v>2</v>
       </c>
@@ -4536,8 +4728,12 @@
         <f>IFERROR(VLOOKUP(_stats[[#This Row],[player_id]],_players[[player_id]:[player_name]],2,0),"")</f>
         <v>Егор (АК+1)</v>
       </c>
-      <c r="E86" s="26"/>
-      <c r="F86" s="28"/>
+      <c r="E86" s="26">
+        <v>0</v>
+      </c>
+      <c r="F86" s="28">
+        <v>0</v>
+      </c>
       <c r="G86" s="27">
         <v>2</v>
       </c>
@@ -4559,7 +4755,9 @@
       <c r="E87" s="26">
         <v>1</v>
       </c>
-      <c r="F87" s="28"/>
+      <c r="F87" s="28">
+        <v>0</v>
+      </c>
       <c r="G87" s="27">
         <v>2</v>
       </c>
@@ -4605,7 +4803,9 @@
       <c r="E89" s="26">
         <v>1</v>
       </c>
-      <c r="F89" s="28"/>
+      <c r="F89" s="28">
+        <v>0</v>
+      </c>
       <c r="G89" s="27">
         <v>4</v>
       </c>
@@ -4631,8 +4831,8 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
30 vs 31_08_2025 3
</commit_message>
<xml_diff>
--- a/football_stats.xlsx
+++ b/football_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\football_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF61906-A176-4340-B774-008D9BAAB335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0428F4-C147-475E-A2FC-AAA15175E35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15450" yWindow="30" windowWidth="13350" windowHeight="14775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1499,11 +1499,11 @@
       </c>
       <c r="E3" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F3" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1571,11 +1571,11 @@
       </c>
       <c r="E6" s="16">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F6" s="17">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1619,11 +1619,11 @@
       </c>
       <c r="E8" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F8" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1667,11 +1667,11 @@
       </c>
       <c r="E10" s="16">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F10" s="17">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1715,11 +1715,11 @@
       </c>
       <c r="E12" s="16">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F12" s="17">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1763,11 +1763,11 @@
       </c>
       <c r="E14" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F14" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1811,11 +1811,11 @@
       </c>
       <c r="E16" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F16" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1859,11 +1859,11 @@
       </c>
       <c r="E18" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F18" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="E20" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F20" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1931,11 +1931,11 @@
       </c>
       <c r="E21" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F21" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2027,11 +2027,11 @@
       </c>
       <c r="E25" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F25" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2099,11 +2099,11 @@
       </c>
       <c r="E28" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F28" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2123,11 +2123,11 @@
       </c>
       <c r="E29" s="16">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F29" s="17">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2195,11 +2195,11 @@
       </c>
       <c r="E32" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F32" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2315,11 +2315,11 @@
       </c>
       <c r="E37" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F37" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2363,11 +2363,11 @@
       </c>
       <c r="E39" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F39" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2387,11 +2387,11 @@
       </c>
       <c r="E40" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F40" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2411,11 +2411,11 @@
       </c>
       <c r="E41" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F41" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2435,11 +2435,11 @@
       </c>
       <c r="E42" s="16">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F42" s="17">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2459,11 +2459,11 @@
       </c>
       <c r="E43" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F43" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2507,11 +2507,11 @@
       </c>
       <c r="E45" s="16">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F45" s="17">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2627,11 +2627,11 @@
       </c>
       <c r="E50" s="11">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F50" s="12">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2795,11 +2795,11 @@
       </c>
       <c r="E57" s="10">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F57" s="18">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2843,11 +2843,11 @@
       </c>
       <c r="E59" s="10">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F59" s="18">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2939,11 +2939,11 @@
       </c>
       <c r="E63" s="10">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F63" s="18">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3059,11 +3059,11 @@
       </c>
       <c r="E68" s="7">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F68" s="8">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3251,11 +3251,11 @@
       </c>
       <c r="E76" s="10">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F76" s="18">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3323,11 +3323,11 @@
       </c>
       <c r="E79" s="10">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F79" s="18">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3515,11 +3515,11 @@
       </c>
       <c r="E87" s="10">
         <f>SUMIFS(_stats[wins_on_date],_stats[player_id],_players[[#This Row],[player_id]])</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F87" s="18">
         <f>SUM(_players[[#This Row],[goals]:[wins]])</f>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3561,7 +3561,7 @@
   </sheetPr>
   <dimension ref="A1:G487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A458" workbookViewId="0">
       <selection activeCell="D466" sqref="D466"/>
     </sheetView>
   </sheetViews>
@@ -15045,7 +15045,7 @@
       </c>
       <c r="G459" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.25">
@@ -15070,7 +15070,7 @@
       </c>
       <c r="G460" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.25">
@@ -15095,7 +15095,7 @@
       </c>
       <c r="G461" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="462" spans="1:7" x14ac:dyDescent="0.25">
@@ -15120,7 +15120,7 @@
       </c>
       <c r="G462" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
@@ -15145,7 +15145,7 @@
       </c>
       <c r="G463" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.25">
@@ -15170,7 +15170,7 @@
       </c>
       <c r="G464" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="465" spans="1:7" x14ac:dyDescent="0.25">
@@ -15195,7 +15195,7 @@
       </c>
       <c r="G465" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="466" spans="1:7" x14ac:dyDescent="0.25">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="G466" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.25">
@@ -15245,7 +15245,7 @@
       </c>
       <c r="G467" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="468" spans="1:7" x14ac:dyDescent="0.25">
@@ -15270,7 +15270,7 @@
       </c>
       <c r="G468" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.25">
@@ -15295,7 +15295,7 @@
       </c>
       <c r="G469" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.25">
@@ -15320,7 +15320,7 @@
       </c>
       <c r="G470" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="471" spans="1:7" x14ac:dyDescent="0.25">
@@ -15345,7 +15345,7 @@
       </c>
       <c r="G471" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="472" spans="1:7" x14ac:dyDescent="0.25">
@@ -15370,7 +15370,7 @@
       </c>
       <c r="G472" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="473" spans="1:7" x14ac:dyDescent="0.25">
@@ -15395,7 +15395,7 @@
       </c>
       <c r="G473" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="474" spans="1:7" x14ac:dyDescent="0.25">
@@ -15420,7 +15420,7 @@
       </c>
       <c r="G474" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="475" spans="1:7" x14ac:dyDescent="0.25">
@@ -15445,7 +15445,7 @@
       </c>
       <c r="G475" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="476" spans="1:7" x14ac:dyDescent="0.25">
@@ -15470,7 +15470,7 @@
       </c>
       <c r="G476" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="477" spans="1:7" x14ac:dyDescent="0.25">
@@ -15495,7 +15495,7 @@
       </c>
       <c r="G477" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="478" spans="1:7" x14ac:dyDescent="0.25">
@@ -15520,7 +15520,7 @@
       </c>
       <c r="G478" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="479" spans="1:7" x14ac:dyDescent="0.25">
@@ -15545,7 +15545,7 @@
       </c>
       <c r="G479" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="480" spans="1:7" x14ac:dyDescent="0.25">
@@ -15570,7 +15570,7 @@
       </c>
       <c r="G480" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="481" spans="1:7" x14ac:dyDescent="0.25">
@@ -15595,7 +15595,7 @@
       </c>
       <c r="G481" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.25">
@@ -15620,7 +15620,7 @@
       </c>
       <c r="G482" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="483" spans="1:7" x14ac:dyDescent="0.25">
@@ -15645,7 +15645,7 @@
       </c>
       <c r="G483" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="484" spans="1:7" x14ac:dyDescent="0.25">
@@ -15670,7 +15670,7 @@
       </c>
       <c r="G484" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="485" spans="1:7" x14ac:dyDescent="0.25">
@@ -15695,7 +15695,7 @@
       </c>
       <c r="G485" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="486" spans="1:7" x14ac:dyDescent="0.25">
@@ -15720,7 +15720,7 @@
       </c>
       <c r="G486" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="487" spans="1:7" x14ac:dyDescent="0.25">
@@ -15745,7 +15745,7 @@
       </c>
       <c r="G487" s="10">
         <f>SUMIFS(_teams[wins_on_date],_teams[date],_stats[[#This Row],[date]],_teams[team_number],_stats[[#This Row],[team_number]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -15771,7 +15771,7 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16542,7 +16542,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
-        <v>45899</v>
+        <v>45900</v>
       </c>
       <c r="B70" s="7">
         <v>1</v>
@@ -16553,7 +16553,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
-        <v>45899</v>
+        <v>45900</v>
       </c>
       <c r="B71" s="7">
         <v>2</v>
@@ -16564,7 +16564,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
-        <v>45899</v>
+        <v>45900</v>
       </c>
       <c r="B72" s="7">
         <v>3</v>
@@ -16575,7 +16575,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
-        <v>45899</v>
+        <v>45900</v>
       </c>
       <c r="B73" s="7">
         <v>4</v>

</xml_diff>